<commit_message>
imdb parsing +xlsx list+enc ver.
</commit_message>
<xml_diff>
--- a/login_attempts.xlsx
+++ b/login_attempts.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -27,12 +27,6 @@
   </si>
   <si>
     <t>Blocked At</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>2025-07-10T03:10:58.284236</t>
   </si>
 </sst>
 </file>
@@ -77,17 +71,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.83984375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="2.9453125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.90234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.1875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.94140625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="29.25" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.47265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -107,23 +101,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>12381.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="D2" t="b" s="0">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>